<commit_message>
continued developing A* algorithm and added mapping criteria
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\python_projects\local_files\a_star\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\python_projects\slam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC7A2878-3F2E-45A7-8BC6-25FE8584E380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB982434-1183-4D39-8D18-49BAFC5897DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="23">
   <si>
     <t>col1</t>
   </si>
@@ -188,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -196,11 +196,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -238,16 +318,67 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -534,12 +665,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -601,7 +732,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -663,7 +794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -725,7 +856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -787,7 +918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -849,7 +980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4">
         <v>0</v>
       </c>
@@ -911,7 +1042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -973,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -1035,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -1097,7 +1228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -1159,7 +1290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3">
         <v>255</v>
       </c>
@@ -1221,7 +1352,7 @@
         <v>-255</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>0</v>
       </c>
@@ -1283,7 +1414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>0</v>
       </c>
@@ -1345,7 +1476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>0</v>
       </c>
@@ -1407,7 +1538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
         <v>0</v>
       </c>
@@ -1469,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
         <v>0</v>
       </c>
@@ -1531,7 +1662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1">
         <v>0</v>
       </c>
@@ -1593,7 +1724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -1655,7 +1786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1">
         <v>0</v>
       </c>
@@ -1717,7 +1848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -1779,7 +1910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1">
         <v>0</v>
       </c>
@@ -1849,18 +1980,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD033E48-BD4B-4984-B655-F119C77DB1ED}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1886,7 +2017,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1912,7 +2043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -1938,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -1964,7 +2095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -1990,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -2016,7 +2147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -2042,7 +2173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -2068,7 +2199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -2094,7 +2225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -2120,7 +2251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -2143,6 +2274,322 @@
         <v>0</v>
       </c>
       <c r="H11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1">
+        <v>0</v>
+      </c>
+      <c r="B15" s="15">
+        <v>0</v>
+      </c>
+      <c r="C15" s="16">
+        <v>0</v>
+      </c>
+      <c r="D15" s="16">
+        <v>0</v>
+      </c>
+      <c r="E15" s="16">
+        <v>0</v>
+      </c>
+      <c r="F15" s="16">
+        <v>0</v>
+      </c>
+      <c r="G15" s="16">
+        <v>0</v>
+      </c>
+      <c r="H15" s="16">
+        <v>0</v>
+      </c>
+      <c r="I15" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="18">
+        <v>0</v>
+      </c>
+      <c r="C16" s="19">
+        <v>0</v>
+      </c>
+      <c r="D16" s="19">
+        <v>0</v>
+      </c>
+      <c r="E16" s="19">
+        <v>0</v>
+      </c>
+      <c r="F16" s="19">
+        <v>0</v>
+      </c>
+      <c r="G16" s="19">
+        <v>0</v>
+      </c>
+      <c r="H16" s="19">
+        <v>0</v>
+      </c>
+      <c r="I16" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="1">
+        <v>2</v>
+      </c>
+      <c r="B17" s="18">
+        <v>0</v>
+      </c>
+      <c r="C17" s="19">
+        <v>0</v>
+      </c>
+      <c r="D17" s="19">
+        <v>0</v>
+      </c>
+      <c r="E17" s="19">
+        <v>0</v>
+      </c>
+      <c r="F17" s="19">
+        <v>0</v>
+      </c>
+      <c r="G17" s="19">
+        <v>0</v>
+      </c>
+      <c r="H17" s="19">
+        <v>0</v>
+      </c>
+      <c r="I17" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="1">
+        <v>3</v>
+      </c>
+      <c r="B18" s="18">
+        <v>0</v>
+      </c>
+      <c r="C18" s="19">
+        <v>0</v>
+      </c>
+      <c r="D18" s="19">
+        <v>0</v>
+      </c>
+      <c r="E18" s="21">
+        <v>0</v>
+      </c>
+      <c r="F18" s="21">
+        <v>0</v>
+      </c>
+      <c r="G18" s="21">
+        <v>0</v>
+      </c>
+      <c r="H18" s="19">
+        <v>0</v>
+      </c>
+      <c r="I18" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="1">
+        <v>4</v>
+      </c>
+      <c r="B19" s="18">
+        <v>0</v>
+      </c>
+      <c r="C19" s="19">
+        <v>0</v>
+      </c>
+      <c r="D19" s="22">
+        <v>0</v>
+      </c>
+      <c r="E19" s="23">
+        <v>0</v>
+      </c>
+      <c r="F19" s="24">
+        <v>1</v>
+      </c>
+      <c r="G19" s="21">
+        <v>0</v>
+      </c>
+      <c r="H19" s="19">
+        <v>0</v>
+      </c>
+      <c r="I19" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="1">
+        <v>5</v>
+      </c>
+      <c r="B20" s="18">
+        <v>0</v>
+      </c>
+      <c r="C20" s="19">
+        <v>0</v>
+      </c>
+      <c r="D20" s="22">
+        <v>0</v>
+      </c>
+      <c r="E20" s="25">
+        <v>0</v>
+      </c>
+      <c r="F20" s="24">
+        <v>1</v>
+      </c>
+      <c r="G20" s="21">
+        <v>0</v>
+      </c>
+      <c r="H20" s="19">
+        <v>0</v>
+      </c>
+      <c r="I20" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="1">
+        <v>6</v>
+      </c>
+      <c r="B21" s="18">
+        <v>0</v>
+      </c>
+      <c r="C21" s="26">
+        <v>255</v>
+      </c>
+      <c r="D21" s="23">
+        <v>0</v>
+      </c>
+      <c r="E21" s="23">
+        <v>0</v>
+      </c>
+      <c r="F21" s="24">
+        <v>1</v>
+      </c>
+      <c r="G21" s="21">
+        <v>0</v>
+      </c>
+      <c r="H21" s="27">
+        <v>-255</v>
+      </c>
+      <c r="I21" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="1">
+        <v>7</v>
+      </c>
+      <c r="B22" s="18">
+        <v>0</v>
+      </c>
+      <c r="C22" s="19">
+        <v>0</v>
+      </c>
+      <c r="D22" s="28">
+        <v>0</v>
+      </c>
+      <c r="E22" s="28">
+        <v>0</v>
+      </c>
+      <c r="F22" s="29">
+        <v>1</v>
+      </c>
+      <c r="G22" s="19">
+        <v>0</v>
+      </c>
+      <c r="H22" s="19">
+        <v>0</v>
+      </c>
+      <c r="I22" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="1">
+        <v>8</v>
+      </c>
+      <c r="B23" s="18">
+        <v>0</v>
+      </c>
+      <c r="C23" s="19">
+        <v>0</v>
+      </c>
+      <c r="D23" s="19">
+        <v>0</v>
+      </c>
+      <c r="E23" s="19">
+        <v>0</v>
+      </c>
+      <c r="F23" s="29">
+        <v>1</v>
+      </c>
+      <c r="G23" s="19">
+        <v>0</v>
+      </c>
+      <c r="H23" s="19">
+        <v>0</v>
+      </c>
+      <c r="I23" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="1">
+        <v>9</v>
+      </c>
+      <c r="B24" s="30">
+        <v>0</v>
+      </c>
+      <c r="C24" s="31">
+        <v>0</v>
+      </c>
+      <c r="D24" s="31">
+        <v>0</v>
+      </c>
+      <c r="E24" s="31">
+        <v>0</v>
+      </c>
+      <c r="F24" s="32">
+        <v>1</v>
+      </c>
+      <c r="G24" s="31">
+        <v>0</v>
+      </c>
+      <c r="H24" s="31">
+        <v>0</v>
+      </c>
+      <c r="I24" s="33">
         <v>0</v>
       </c>
     </row>
@@ -2159,12 +2606,12 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -2190,7 +2637,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2216,7 +2663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -2242,7 +2689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -2268,7 +2715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -2294,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -2320,7 +2767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -2346,7 +2793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -2372,7 +2819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -2398,7 +2845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -2424,7 +2871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -2464,12 +2911,12 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -2492,7 +2939,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2515,7 +2962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -2538,7 +2985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -2561,7 +3008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -2584,7 +3031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -2607,7 +3054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -2630,7 +3077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -2666,12 +3113,12 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -2694,7 +3141,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2717,7 +3164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -2740,7 +3187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -2763,7 +3210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -2786,7 +3233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -2809,7 +3256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -2841,16 +3288,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA649F3C-9117-4912-8352-7DDFBD834BCF}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -2870,7 +3317,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2890,7 +3337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -2910,7 +3357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -2920,7 +3367,7 @@
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="4">
         <v>0</v>
       </c>
       <c r="E4" s="1">
@@ -2930,7 +3377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -2950,7 +3397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -2970,7 +3417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -3001,12 +3448,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -3044,7 +3491,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3085,7 +3532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -3126,7 +3573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -3167,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -3195,20 +3642,20 @@
       <c r="I5" s="1">
         <v>0</v>
       </c>
-      <c r="J5" s="13">
-        <v>0</v>
-      </c>
-      <c r="K5" s="13">
-        <v>0</v>
-      </c>
-      <c r="L5" s="13">
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
         <v>0</v>
       </c>
       <c r="M5" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -3236,20 +3683,20 @@
       <c r="I6" s="6">
         <v>0</v>
       </c>
-      <c r="J6" s="13">
-        <v>0</v>
-      </c>
-      <c r="K6" s="13">
-        <v>0</v>
-      </c>
-      <c r="L6" s="13">
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
         <v>0</v>
       </c>
       <c r="M6" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -3262,35 +3709,35 @@
       <c r="D7" s="6">
         <v>0</v>
       </c>
-      <c r="E7" s="15">
-        <v>1</v>
-      </c>
-      <c r="F7" s="15">
-        <v>1</v>
-      </c>
-      <c r="G7" s="15">
-        <v>1</v>
-      </c>
-      <c r="H7" s="15">
-        <v>1</v>
-      </c>
-      <c r="I7" s="15">
+      <c r="E7" s="13">
+        <v>1</v>
+      </c>
+      <c r="F7" s="13">
+        <v>1</v>
+      </c>
+      <c r="G7" s="13">
+        <v>1</v>
+      </c>
+      <c r="H7" s="13">
+        <v>1</v>
+      </c>
+      <c r="I7" s="13">
         <v>1</v>
       </c>
       <c r="J7" s="12">
         <v>0</v>
       </c>
-      <c r="K7" s="16">
-        <v>0</v>
-      </c>
-      <c r="L7" s="13">
+      <c r="K7" s="14">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
         <v>0</v>
       </c>
       <c r="M7" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -3300,28 +3747,28 @@
       <c r="C8" s="6">
         <v>0</v>
       </c>
-      <c r="D8" s="15">
-        <v>1</v>
-      </c>
-      <c r="E8" s="15">
-        <v>1</v>
-      </c>
-      <c r="F8" s="15">
-        <v>1</v>
-      </c>
-      <c r="G8" s="15">
-        <v>1</v>
-      </c>
-      <c r="H8" s="15">
-        <v>1</v>
-      </c>
-      <c r="I8" s="15">
-        <v>1</v>
-      </c>
-      <c r="J8" s="15">
-        <v>1</v>
-      </c>
-      <c r="K8" s="14">
+      <c r="D8" s="13">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13">
+        <v>1</v>
+      </c>
+      <c r="F8" s="13">
+        <v>1</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>1</v>
+      </c>
+      <c r="I8" s="13">
+        <v>1</v>
+      </c>
+      <c r="J8" s="13">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1">
         <v>0</v>
       </c>
       <c r="L8" s="5">
@@ -3331,7 +3778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -3356,7 +3803,7 @@
       <c r="H9" s="4">
         <v>0</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="4">
         <v>0</v>
       </c>
       <c r="J9" s="1">
@@ -3372,7 +3819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -3397,7 +3844,7 @@
       <c r="H10" s="1">
         <v>0</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="4">
         <v>0</v>
       </c>
       <c r="J10" s="1">
@@ -3413,7 +3860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -3438,7 +3885,7 @@
       <c r="H11" s="1">
         <v>0</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="4">
         <v>0</v>
       </c>
       <c r="J11" s="1">
@@ -3468,12 +3915,12 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -3511,7 +3958,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3549,7 +3996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -3587,7 +4034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -3625,7 +4072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -3656,14 +4103,14 @@
       <c r="J5" s="1">
         <v>0</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="4">
         <v>0</v>
       </c>
       <c r="L5" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -3694,14 +4141,14 @@
       <c r="J6" s="1">
         <v>0</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="4">
         <v>0</v>
       </c>
       <c r="L6" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -3732,14 +4179,14 @@
       <c r="J7" s="1">
         <v>0</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="4">
         <v>0</v>
       </c>
       <c r="L7" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -3777,7 +4224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -3815,7 +4262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -3840,7 +4287,7 @@
       <c r="H10" s="1">
         <v>0</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="4">
         <v>0</v>
       </c>
       <c r="J10" s="1">
@@ -3853,7 +4300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -3878,7 +4325,7 @@
       <c r="H11" s="1">
         <v>0</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="4">
         <v>0</v>
       </c>
       <c r="J11" s="1">
@@ -3904,12 +4351,12 @@
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -3947,7 +4394,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3985,7 +4432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -4023,7 +4470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -4061,7 +4508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -4092,14 +4539,14 @@
       <c r="J5" s="1">
         <v>0</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="4">
         <v>0</v>
       </c>
       <c r="L5" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -4130,14 +4577,14 @@
       <c r="J6" s="1">
         <v>0</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="4">
         <v>0</v>
       </c>
       <c r="L6" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -4168,14 +4615,14 @@
       <c r="J7" s="2">
         <v>1</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="4">
         <v>0</v>
       </c>
       <c r="L7" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -4213,7 +4660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -4251,7 +4698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -4289,7 +4736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -4314,7 +4761,7 @@
       <c r="H11" s="1">
         <v>0</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="4">
         <v>0</v>
       </c>
       <c r="J11" s="1">

</xml_diff>

<commit_message>
added map visualization, edited get_kernel_min method in a_star class
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\python_projects\slam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB982434-1183-4D39-8D18-49BAFC5897DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E7AC60-620F-4E5D-896C-45F6905A485D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="23">
   <si>
     <t>col1</t>
   </si>
@@ -188,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -196,91 +196,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -322,63 +242,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -663,14 +526,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -732,7 +597,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -794,7 +659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -856,7 +721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -918,7 +783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -980,7 +845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>0</v>
       </c>
@@ -1042,7 +907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -1104,7 +969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -1166,7 +1031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -1228,7 +1093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -1290,7 +1155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>255</v>
       </c>
@@ -1352,7 +1217,7 @@
         <v>-255</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0</v>
       </c>
@@ -1414,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0</v>
       </c>
@@ -1476,7 +1341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0</v>
       </c>
@@ -1538,7 +1403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>0</v>
       </c>
@@ -1600,7 +1465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0</v>
       </c>
@@ -1662,7 +1527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>0</v>
       </c>
@@ -1724,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -1786,7 +1651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>0</v>
       </c>
@@ -1848,7 +1713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -1910,7 +1775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>0</v>
       </c>
@@ -1980,18 +1845,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD033E48-BD4B-4984-B655-F119C77DB1ED}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -2017,7 +1880,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2043,7 +1906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -2069,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -2095,7 +1958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -2121,7 +1984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -2147,7 +2010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -2173,7 +2036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -2199,7 +2062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -2225,7 +2088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -2251,7 +2114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -2274,322 +2137,6 @@
         <v>0</v>
       </c>
       <c r="H11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="1">
-        <v>0</v>
-      </c>
-      <c r="B15" s="15">
-        <v>0</v>
-      </c>
-      <c r="C15" s="16">
-        <v>0</v>
-      </c>
-      <c r="D15" s="16">
-        <v>0</v>
-      </c>
-      <c r="E15" s="16">
-        <v>0</v>
-      </c>
-      <c r="F15" s="16">
-        <v>0</v>
-      </c>
-      <c r="G15" s="16">
-        <v>0</v>
-      </c>
-      <c r="H15" s="16">
-        <v>0</v>
-      </c>
-      <c r="I15" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="1">
-        <v>1</v>
-      </c>
-      <c r="B16" s="18">
-        <v>0</v>
-      </c>
-      <c r="C16" s="19">
-        <v>0</v>
-      </c>
-      <c r="D16" s="19">
-        <v>0</v>
-      </c>
-      <c r="E16" s="19">
-        <v>0</v>
-      </c>
-      <c r="F16" s="19">
-        <v>0</v>
-      </c>
-      <c r="G16" s="19">
-        <v>0</v>
-      </c>
-      <c r="H16" s="19">
-        <v>0</v>
-      </c>
-      <c r="I16" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="1">
-        <v>2</v>
-      </c>
-      <c r="B17" s="18">
-        <v>0</v>
-      </c>
-      <c r="C17" s="19">
-        <v>0</v>
-      </c>
-      <c r="D17" s="19">
-        <v>0</v>
-      </c>
-      <c r="E17" s="19">
-        <v>0</v>
-      </c>
-      <c r="F17" s="19">
-        <v>0</v>
-      </c>
-      <c r="G17" s="19">
-        <v>0</v>
-      </c>
-      <c r="H17" s="19">
-        <v>0</v>
-      </c>
-      <c r="I17" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="1">
-        <v>3</v>
-      </c>
-      <c r="B18" s="18">
-        <v>0</v>
-      </c>
-      <c r="C18" s="19">
-        <v>0</v>
-      </c>
-      <c r="D18" s="19">
-        <v>0</v>
-      </c>
-      <c r="E18" s="21">
-        <v>0</v>
-      </c>
-      <c r="F18" s="21">
-        <v>0</v>
-      </c>
-      <c r="G18" s="21">
-        <v>0</v>
-      </c>
-      <c r="H18" s="19">
-        <v>0</v>
-      </c>
-      <c r="I18" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="1">
-        <v>4</v>
-      </c>
-      <c r="B19" s="18">
-        <v>0</v>
-      </c>
-      <c r="C19" s="19">
-        <v>0</v>
-      </c>
-      <c r="D19" s="22">
-        <v>0</v>
-      </c>
-      <c r="E19" s="23">
-        <v>0</v>
-      </c>
-      <c r="F19" s="24">
-        <v>1</v>
-      </c>
-      <c r="G19" s="21">
-        <v>0</v>
-      </c>
-      <c r="H19" s="19">
-        <v>0</v>
-      </c>
-      <c r="I19" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="1">
-        <v>5</v>
-      </c>
-      <c r="B20" s="18">
-        <v>0</v>
-      </c>
-      <c r="C20" s="19">
-        <v>0</v>
-      </c>
-      <c r="D20" s="22">
-        <v>0</v>
-      </c>
-      <c r="E20" s="25">
-        <v>0</v>
-      </c>
-      <c r="F20" s="24">
-        <v>1</v>
-      </c>
-      <c r="G20" s="21">
-        <v>0</v>
-      </c>
-      <c r="H20" s="19">
-        <v>0</v>
-      </c>
-      <c r="I20" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="1">
-        <v>6</v>
-      </c>
-      <c r="B21" s="18">
-        <v>0</v>
-      </c>
-      <c r="C21" s="26">
-        <v>255</v>
-      </c>
-      <c r="D21" s="23">
-        <v>0</v>
-      </c>
-      <c r="E21" s="23">
-        <v>0</v>
-      </c>
-      <c r="F21" s="24">
-        <v>1</v>
-      </c>
-      <c r="G21" s="21">
-        <v>0</v>
-      </c>
-      <c r="H21" s="27">
-        <v>-255</v>
-      </c>
-      <c r="I21" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="1">
-        <v>7</v>
-      </c>
-      <c r="B22" s="18">
-        <v>0</v>
-      </c>
-      <c r="C22" s="19">
-        <v>0</v>
-      </c>
-      <c r="D22" s="28">
-        <v>0</v>
-      </c>
-      <c r="E22" s="28">
-        <v>0</v>
-      </c>
-      <c r="F22" s="29">
-        <v>1</v>
-      </c>
-      <c r="G22" s="19">
-        <v>0</v>
-      </c>
-      <c r="H22" s="19">
-        <v>0</v>
-      </c>
-      <c r="I22" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="1">
-        <v>8</v>
-      </c>
-      <c r="B23" s="18">
-        <v>0</v>
-      </c>
-      <c r="C23" s="19">
-        <v>0</v>
-      </c>
-      <c r="D23" s="19">
-        <v>0</v>
-      </c>
-      <c r="E23" s="19">
-        <v>0</v>
-      </c>
-      <c r="F23" s="29">
-        <v>1</v>
-      </c>
-      <c r="G23" s="19">
-        <v>0</v>
-      </c>
-      <c r="H23" s="19">
-        <v>0</v>
-      </c>
-      <c r="I23" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="1">
-        <v>9</v>
-      </c>
-      <c r="B24" s="30">
-        <v>0</v>
-      </c>
-      <c r="C24" s="31">
-        <v>0</v>
-      </c>
-      <c r="D24" s="31">
-        <v>0</v>
-      </c>
-      <c r="E24" s="31">
-        <v>0</v>
-      </c>
-      <c r="F24" s="32">
-        <v>1</v>
-      </c>
-      <c r="G24" s="31">
-        <v>0</v>
-      </c>
-      <c r="H24" s="31">
-        <v>0</v>
-      </c>
-      <c r="I24" s="33">
         <v>0</v>
       </c>
     </row>
@@ -2606,12 +2153,12 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -2637,7 +2184,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2663,7 +2210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -2689,7 +2236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -2715,7 +2262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -2741,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -2767,7 +2314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -2793,7 +2340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -2819,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -2845,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -2871,7 +2418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -2908,15 +2455,15 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -2939,7 +2486,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2962,7 +2509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -2985,7 +2532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -3008,7 +2555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -3031,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -3054,7 +2601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -3077,7 +2624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -3113,12 +2660,12 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -3141,7 +2688,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3164,7 +2711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -3187,7 +2734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -3210,7 +2757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -3233,7 +2780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -3256,7 +2803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -3289,15 +2836,15 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -3317,7 +2864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3337,14 +2884,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3" s="8">
         <v>-255</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="6">
         <v>0</v>
       </c>
       <c r="D3" s="1">
@@ -3357,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -3367,7 +2914,7 @@
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="12">
         <v>0</v>
       </c>
       <c r="E4" s="1">
@@ -3377,7 +2924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -3387,17 +2934,17 @@
       <c r="C5" s="1">
         <v>0</v>
       </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6">
         <v>0</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -3417,7 +2964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -3448,12 +2995,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -3491,7 +3038,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3532,7 +3079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -3573,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -3614,7 +3161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -3655,7 +3202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -3696,7 +3243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -3737,7 +3284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -3778,7 +3325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -3819,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -3860,7 +3407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -3915,12 +3462,12 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -3958,7 +3505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3996,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -4034,7 +3581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -4072,7 +3619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -4110,7 +3657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -4148,7 +3695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -4186,7 +3733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -4224,7 +3771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -4262,7 +3809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -4300,7 +3847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -4347,16 +3894,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51333FAB-9D50-443F-9322-F9DDD983843B}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -4394,7 +3941,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4432,7 +3979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -4470,7 +4017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -4508,7 +4055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -4546,7 +4093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -4584,7 +4131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -4622,7 +4169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -4660,7 +4207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -4698,7 +4245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -4736,7 +4283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
added more test maps
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\python_projects\slam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E7AC60-620F-4E5D-896C-45F6905A485D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF6BD3D-D4F1-41CE-A703-58778B235DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,8 @@
     <sheet name="Sheet7" sheetId="9" r:id="rId7"/>
     <sheet name="Sheet8" sheetId="10" r:id="rId8"/>
     <sheet name="Sheet9" sheetId="11" r:id="rId9"/>
+    <sheet name="Sheet10" sheetId="12" r:id="rId10"/>
+    <sheet name="Sheet11" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="28">
   <si>
     <t>col1</t>
   </si>
@@ -102,6 +104,21 @@
   </si>
   <si>
     <t>col0</t>
+  </si>
+  <si>
+    <t>col21</t>
+  </si>
+  <si>
+    <t>col22</t>
+  </si>
+  <si>
+    <t>col23</t>
+  </si>
+  <si>
+    <t>col24</t>
+  </si>
+  <si>
+    <t>col25</t>
   </si>
 </sst>
 </file>
@@ -200,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -244,6 +261,10 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1843,6 +1864,2941 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53924B42-3909-4272-A548-B312509CF1B3}">
+  <dimension ref="A1:Z20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="26" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="16">
+        <v>1</v>
+      </c>
+      <c r="D3" s="16">
+        <v>1</v>
+      </c>
+      <c r="E3" s="16">
+        <v>1</v>
+      </c>
+      <c r="F3" s="16">
+        <v>1</v>
+      </c>
+      <c r="G3" s="16">
+        <v>1</v>
+      </c>
+      <c r="H3" s="16">
+        <v>1</v>
+      </c>
+      <c r="I3" s="16">
+        <v>1</v>
+      </c>
+      <c r="J3" s="16">
+        <v>1</v>
+      </c>
+      <c r="K3" s="16">
+        <v>1</v>
+      </c>
+      <c r="L3" s="16">
+        <v>1</v>
+      </c>
+      <c r="M3" s="16">
+        <v>1</v>
+      </c>
+      <c r="N3" s="16">
+        <v>1</v>
+      </c>
+      <c r="O3" s="16">
+        <v>1</v>
+      </c>
+      <c r="P3" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="16">
+        <v>1</v>
+      </c>
+      <c r="R3" s="16">
+        <v>1</v>
+      </c>
+      <c r="S3" s="16">
+        <v>1</v>
+      </c>
+      <c r="T3" s="16">
+        <v>1</v>
+      </c>
+      <c r="U3" s="16">
+        <v>1</v>
+      </c>
+      <c r="V3" s="16">
+        <v>1</v>
+      </c>
+      <c r="W3" s="16">
+        <v>1</v>
+      </c>
+      <c r="X3" s="16">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="16">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="16">
+        <v>1</v>
+      </c>
+      <c r="D4" s="16">
+        <v>1</v>
+      </c>
+      <c r="E4" s="16">
+        <v>1</v>
+      </c>
+      <c r="F4" s="16">
+        <v>1</v>
+      </c>
+      <c r="G4" s="16">
+        <v>1</v>
+      </c>
+      <c r="H4" s="16">
+        <v>1</v>
+      </c>
+      <c r="I4" s="16">
+        <v>1</v>
+      </c>
+      <c r="J4" s="16">
+        <v>1</v>
+      </c>
+      <c r="K4" s="16">
+        <v>1</v>
+      </c>
+      <c r="L4" s="16">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="16">
+        <v>1</v>
+      </c>
+      <c r="R4" s="16">
+        <v>1</v>
+      </c>
+      <c r="S4" s="16">
+        <v>1</v>
+      </c>
+      <c r="T4" s="16">
+        <v>1</v>
+      </c>
+      <c r="U4" s="16">
+        <v>1</v>
+      </c>
+      <c r="V4" s="16">
+        <v>1</v>
+      </c>
+      <c r="W4" s="16">
+        <v>1</v>
+      </c>
+      <c r="X4" s="16">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="16">
+        <v>1</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="16">
+        <v>1</v>
+      </c>
+      <c r="D5" s="16">
+        <v>1</v>
+      </c>
+      <c r="E5" s="16">
+        <v>1</v>
+      </c>
+      <c r="F5" s="16">
+        <v>1</v>
+      </c>
+      <c r="G5" s="16">
+        <v>1</v>
+      </c>
+      <c r="H5" s="16">
+        <v>1</v>
+      </c>
+      <c r="I5" s="16">
+        <v>1</v>
+      </c>
+      <c r="J5" s="16">
+        <v>1</v>
+      </c>
+      <c r="K5" s="16">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="15">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="16">
+        <v>1</v>
+      </c>
+      <c r="R5" s="16">
+        <v>1</v>
+      </c>
+      <c r="S5" s="16">
+        <v>1</v>
+      </c>
+      <c r="T5" s="16">
+        <v>1</v>
+      </c>
+      <c r="U5" s="16">
+        <v>1</v>
+      </c>
+      <c r="V5" s="16">
+        <v>1</v>
+      </c>
+      <c r="W5" s="16">
+        <v>1</v>
+      </c>
+      <c r="X5" s="16">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="16">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="16">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16">
+        <v>1</v>
+      </c>
+      <c r="E6" s="16">
+        <v>1</v>
+      </c>
+      <c r="F6" s="16">
+        <v>1</v>
+      </c>
+      <c r="G6" s="16">
+        <v>1</v>
+      </c>
+      <c r="H6" s="16">
+        <v>1</v>
+      </c>
+      <c r="I6" s="16">
+        <v>1</v>
+      </c>
+      <c r="J6" s="16">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="16">
+        <v>1</v>
+      </c>
+      <c r="N6" s="16">
+        <v>1</v>
+      </c>
+      <c r="O6" s="16">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6" s="16">
+        <v>1</v>
+      </c>
+      <c r="S6" s="16">
+        <v>1</v>
+      </c>
+      <c r="T6" s="16">
+        <v>1</v>
+      </c>
+      <c r="U6" s="16">
+        <v>1</v>
+      </c>
+      <c r="V6" s="16">
+        <v>1</v>
+      </c>
+      <c r="W6" s="16">
+        <v>1</v>
+      </c>
+      <c r="X6" s="16">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="16">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="16">
+        <v>1</v>
+      </c>
+      <c r="D7" s="16">
+        <v>1</v>
+      </c>
+      <c r="E7" s="16">
+        <v>1</v>
+      </c>
+      <c r="F7" s="16">
+        <v>1</v>
+      </c>
+      <c r="G7" s="16">
+        <v>1</v>
+      </c>
+      <c r="H7" s="16">
+        <v>1</v>
+      </c>
+      <c r="I7" s="16">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="16">
+        <v>1</v>
+      </c>
+      <c r="M7" s="16">
+        <v>1</v>
+      </c>
+      <c r="N7" s="16">
+        <v>1</v>
+      </c>
+      <c r="O7" s="16">
+        <v>1</v>
+      </c>
+      <c r="P7" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7" s="16">
+        <v>1</v>
+      </c>
+      <c r="T7" s="16">
+        <v>1</v>
+      </c>
+      <c r="U7" s="16">
+        <v>1</v>
+      </c>
+      <c r="V7" s="16">
+        <v>1</v>
+      </c>
+      <c r="W7" s="16">
+        <v>1</v>
+      </c>
+      <c r="X7" s="16">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="16">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="16">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16">
+        <v>1</v>
+      </c>
+      <c r="E8" s="16">
+        <v>1</v>
+      </c>
+      <c r="F8" s="16">
+        <v>1</v>
+      </c>
+      <c r="G8" s="16">
+        <v>1</v>
+      </c>
+      <c r="H8" s="16">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8" s="16">
+        <v>1</v>
+      </c>
+      <c r="L8" s="16">
+        <v>1</v>
+      </c>
+      <c r="M8" s="16">
+        <v>1</v>
+      </c>
+      <c r="N8" s="16">
+        <v>1</v>
+      </c>
+      <c r="O8" s="16">
+        <v>1</v>
+      </c>
+      <c r="P8" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="16">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8" s="16">
+        <v>1</v>
+      </c>
+      <c r="U8" s="16">
+        <v>1</v>
+      </c>
+      <c r="V8" s="16">
+        <v>1</v>
+      </c>
+      <c r="W8" s="16">
+        <v>1</v>
+      </c>
+      <c r="X8" s="16">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="16">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="16">
+        <v>1</v>
+      </c>
+      <c r="D9" s="16">
+        <v>1</v>
+      </c>
+      <c r="E9" s="16">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16">
+        <v>1</v>
+      </c>
+      <c r="G9" s="16">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="16">
+        <v>1</v>
+      </c>
+      <c r="K9" s="16">
+        <v>1</v>
+      </c>
+      <c r="L9" s="16">
+        <v>1</v>
+      </c>
+      <c r="M9" s="16">
+        <v>1</v>
+      </c>
+      <c r="N9" s="16">
+        <v>1</v>
+      </c>
+      <c r="O9" s="16">
+        <v>1</v>
+      </c>
+      <c r="P9" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="16">
+        <v>1</v>
+      </c>
+      <c r="R9" s="16">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9" s="16">
+        <v>1</v>
+      </c>
+      <c r="V9" s="16">
+        <v>1</v>
+      </c>
+      <c r="W9" s="16">
+        <v>1</v>
+      </c>
+      <c r="X9" s="16">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="16">
+        <v>1</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="16">
+        <v>1</v>
+      </c>
+      <c r="D10" s="16">
+        <v>1</v>
+      </c>
+      <c r="E10" s="16">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="16">
+        <v>1</v>
+      </c>
+      <c r="J10" s="16">
+        <v>1</v>
+      </c>
+      <c r="K10" s="16">
+        <v>1</v>
+      </c>
+      <c r="L10" s="16">
+        <v>1</v>
+      </c>
+      <c r="M10" s="16">
+        <v>1</v>
+      </c>
+      <c r="N10" s="16">
+        <v>1</v>
+      </c>
+      <c r="O10" s="16">
+        <v>1</v>
+      </c>
+      <c r="P10" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="16">
+        <v>1</v>
+      </c>
+      <c r="R10" s="16">
+        <v>1</v>
+      </c>
+      <c r="S10" s="16">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10" s="16">
+        <v>1</v>
+      </c>
+      <c r="W10" s="16">
+        <v>1</v>
+      </c>
+      <c r="X10" s="16">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="16">
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" s="16">
+        <v>1</v>
+      </c>
+      <c r="D11" s="16">
+        <v>1</v>
+      </c>
+      <c r="E11" s="16">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="16">
+        <v>1</v>
+      </c>
+      <c r="I11" s="16">
+        <v>1</v>
+      </c>
+      <c r="J11" s="16">
+        <v>1</v>
+      </c>
+      <c r="K11" s="16">
+        <v>1</v>
+      </c>
+      <c r="L11" s="16">
+        <v>1</v>
+      </c>
+      <c r="M11" s="16">
+        <v>1</v>
+      </c>
+      <c r="N11" s="16">
+        <v>1</v>
+      </c>
+      <c r="O11" s="16">
+        <v>1</v>
+      </c>
+      <c r="P11" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="16">
+        <v>1</v>
+      </c>
+      <c r="R11" s="16">
+        <v>1</v>
+      </c>
+      <c r="S11" s="16">
+        <v>1</v>
+      </c>
+      <c r="T11" s="16">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11" s="16">
+        <v>1</v>
+      </c>
+      <c r="X11" s="16">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="16">
+        <v>1</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="16">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="16">
+        <v>1</v>
+      </c>
+      <c r="H12" s="16">
+        <v>1</v>
+      </c>
+      <c r="I12" s="16">
+        <v>1</v>
+      </c>
+      <c r="J12" s="16">
+        <v>1</v>
+      </c>
+      <c r="K12" s="16">
+        <v>1</v>
+      </c>
+      <c r="L12" s="16">
+        <v>1</v>
+      </c>
+      <c r="M12" s="16">
+        <v>1</v>
+      </c>
+      <c r="N12" s="16">
+        <v>1</v>
+      </c>
+      <c r="O12" s="16">
+        <v>1</v>
+      </c>
+      <c r="P12" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="16">
+        <v>1</v>
+      </c>
+      <c r="R12" s="16">
+        <v>1</v>
+      </c>
+      <c r="S12" s="16">
+        <v>1</v>
+      </c>
+      <c r="T12" s="16">
+        <v>1</v>
+      </c>
+      <c r="U12" s="16">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12" s="16">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="16">
+        <v>1</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" s="16">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="16">
+        <v>1</v>
+      </c>
+      <c r="G13" s="16">
+        <v>1</v>
+      </c>
+      <c r="H13" s="16">
+        <v>1</v>
+      </c>
+      <c r="I13" s="16">
+        <v>1</v>
+      </c>
+      <c r="J13" s="16">
+        <v>1</v>
+      </c>
+      <c r="K13" s="16">
+        <v>1</v>
+      </c>
+      <c r="L13" s="16">
+        <v>1</v>
+      </c>
+      <c r="M13" s="16">
+        <v>1</v>
+      </c>
+      <c r="N13" s="16">
+        <v>1</v>
+      </c>
+      <c r="O13" s="16">
+        <v>1</v>
+      </c>
+      <c r="P13" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="16">
+        <v>1</v>
+      </c>
+      <c r="R13" s="16">
+        <v>1</v>
+      </c>
+      <c r="S13" s="16">
+        <v>1</v>
+      </c>
+      <c r="T13" s="16">
+        <v>1</v>
+      </c>
+      <c r="U13" s="16">
+        <v>1</v>
+      </c>
+      <c r="V13" s="16">
+        <v>1</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="16">
+        <v>1</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="16">
+        <v>1</v>
+      </c>
+      <c r="D14" s="18">
+        <v>255</v>
+      </c>
+      <c r="E14" s="16">
+        <v>1</v>
+      </c>
+      <c r="F14" s="16">
+        <v>1</v>
+      </c>
+      <c r="G14" s="16">
+        <v>1</v>
+      </c>
+      <c r="H14" s="16">
+        <v>1</v>
+      </c>
+      <c r="I14" s="16">
+        <v>1</v>
+      </c>
+      <c r="J14" s="16">
+        <v>1</v>
+      </c>
+      <c r="K14" s="16">
+        <v>1</v>
+      </c>
+      <c r="L14" s="16">
+        <v>1</v>
+      </c>
+      <c r="M14" s="16">
+        <v>1</v>
+      </c>
+      <c r="N14" s="16">
+        <v>1</v>
+      </c>
+      <c r="O14" s="16">
+        <v>1</v>
+      </c>
+      <c r="P14" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="16">
+        <v>1</v>
+      </c>
+      <c r="R14" s="16">
+        <v>1</v>
+      </c>
+      <c r="S14" s="16">
+        <v>1</v>
+      </c>
+      <c r="T14" s="16">
+        <v>1</v>
+      </c>
+      <c r="U14" s="16">
+        <v>1</v>
+      </c>
+      <c r="V14" s="16">
+        <v>1</v>
+      </c>
+      <c r="W14" s="16">
+        <v>1</v>
+      </c>
+      <c r="X14" s="17">
+        <v>-255</v>
+      </c>
+      <c r="Y14" s="16">
+        <v>1</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" s="16">
+        <v>1</v>
+      </c>
+      <c r="D15" s="16">
+        <v>1</v>
+      </c>
+      <c r="E15" s="16">
+        <v>1</v>
+      </c>
+      <c r="F15" s="16">
+        <v>1</v>
+      </c>
+      <c r="G15" s="16">
+        <v>1</v>
+      </c>
+      <c r="H15" s="16">
+        <v>1</v>
+      </c>
+      <c r="I15" s="16">
+        <v>1</v>
+      </c>
+      <c r="J15" s="16">
+        <v>1</v>
+      </c>
+      <c r="K15" s="16">
+        <v>1</v>
+      </c>
+      <c r="L15" s="16">
+        <v>1</v>
+      </c>
+      <c r="M15" s="16">
+        <v>1</v>
+      </c>
+      <c r="N15" s="16">
+        <v>1</v>
+      </c>
+      <c r="O15" s="16">
+        <v>1</v>
+      </c>
+      <c r="P15" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="16">
+        <v>1</v>
+      </c>
+      <c r="R15" s="16">
+        <v>1</v>
+      </c>
+      <c r="S15" s="16">
+        <v>1</v>
+      </c>
+      <c r="T15" s="16">
+        <v>1</v>
+      </c>
+      <c r="U15" s="16">
+        <v>1</v>
+      </c>
+      <c r="V15" s="16">
+        <v>1</v>
+      </c>
+      <c r="W15" s="16">
+        <v>1</v>
+      </c>
+      <c r="X15" s="16">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="16">
+        <v>1</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34EDB805-B65E-44FA-9E03-634BCBD8A426}">
+  <dimension ref="A1:T21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2">
+        <v>1</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>1</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0</v>
+      </c>
+      <c r="S8" s="1">
+        <v>0</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0</v>
+      </c>
+      <c r="R10" s="2">
+        <v>1</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>255</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2">
+        <v>1</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0</v>
+      </c>
+      <c r="T11" s="5">
+        <v>-255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0</v>
+      </c>
+      <c r="R12" s="2">
+        <v>1</v>
+      </c>
+      <c r="S12" s="1">
+        <v>0</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>1</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>0</v>
+      </c>
+      <c r="R13" s="2">
+        <v>1</v>
+      </c>
+      <c r="S13" s="1">
+        <v>0</v>
+      </c>
+      <c r="T13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2">
+        <v>1</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2">
+        <v>1</v>
+      </c>
+      <c r="S14" s="1">
+        <v>0</v>
+      </c>
+      <c r="T14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2">
+        <v>1</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>0</v>
+      </c>
+      <c r="R15" s="1">
+        <v>0</v>
+      </c>
+      <c r="S15" s="1">
+        <v>0</v>
+      </c>
+      <c r="T15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0</v>
+      </c>
+      <c r="M16" s="2">
+        <v>1</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <v>0</v>
+      </c>
+      <c r="P16" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>0</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0</v>
+      </c>
+      <c r="T16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2">
+        <v>1</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1">
+        <v>0</v>
+      </c>
+      <c r="P17" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>0</v>
+      </c>
+      <c r="R17" s="1">
+        <v>0</v>
+      </c>
+      <c r="S17" s="1">
+        <v>0</v>
+      </c>
+      <c r="T17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <v>1</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="2">
+        <v>1</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>0</v>
+      </c>
+      <c r="P18" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>0</v>
+      </c>
+      <c r="R18" s="2">
+        <v>1</v>
+      </c>
+      <c r="S18" s="1">
+        <v>0</v>
+      </c>
+      <c r="T18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1">
+        <v>0</v>
+      </c>
+      <c r="P19" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>0</v>
+      </c>
+      <c r="R19" s="2">
+        <v>1</v>
+      </c>
+      <c r="S19" s="1">
+        <v>0</v>
+      </c>
+      <c r="T19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1">
+        <v>0</v>
+      </c>
+      <c r="P20" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>0</v>
+      </c>
+      <c r="R20" s="2">
+        <v>1</v>
+      </c>
+      <c r="S20" s="1">
+        <v>0</v>
+      </c>
+      <c r="T20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
+        <v>0</v>
+      </c>
+      <c r="P21" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>0</v>
+      </c>
+      <c r="R21" s="2">
+        <v>1</v>
+      </c>
+      <c r="S21" s="1">
+        <v>0</v>
+      </c>
+      <c r="T21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD033E48-BD4B-4984-B655-F119C77DB1ED}">
   <dimension ref="A1:H11"/>
@@ -3894,9 +6850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51333FAB-9D50-443F-9322-F9DDD983843B}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>